<commit_message>
Updated charts with data for Dec. 2025 + plus annotation changes
</commit_message>
<xml_diff>
--- a/visuals/2025-12-israel-tourist-arrivals-by-continent/data/israel_tourist_arrivals.xlsx
+++ b/visuals/2025-12-israel-tourist-arrivals-by-continent/data/israel_tourist_arrivals.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="168">
   <si>
     <t>Topic: Tourism and Accomodations Services</t>
   </si>
@@ -27,7 +27,7 @@
     <t>Value: Tourist Arrivals by Continent and Country of Citizenship</t>
   </si>
   <si>
-    <t>Series Name: Asia,total, Africa,total, Europe,total, NorthAmerica,total, Central America, total, South America,total, Oceania, total</t>
+    <t>Series Name: Asia,total, Uzbekistan, Azerbaijan, United Arab Emirates, Indonesia, Armenia, Georgia, India, Hong Kong, Philippines, Vietnam, Turkey, Taiwan, Japan, Jordan, Malaysia, Nepal, China, Singapore, South Korea, Kazakhstan, Cambodia, Cyprus, Thailand, Asia,Othercountries, Africa,total, Uganda, Ethiopia, Ghana, SouthAfrica, Zimbabwe, IvoryCoast, Tanzania, Mauritius, Egypt, Morocco, Nigeria, Kenya, Rwanda, Tunisia, Africa,Other countries, Europe,total, Austria, Ukraine, Italy, Ireland, Albania, Estonia, Bulgaria, Belgium, Belarus, Germany, Denmark, Netherlands, Hungary, United Kingdom, Greece, Luxembourg, Latvia, Lithuania, Moldova, Montenegro, Malta, Macedonia, Norway, Slovenia, Slovakia, Spain, Serbia, Poland, Portugal, Finland, Czech Republic, France, Croatia, Romania, Russian Federation, Sweden, Switzerland, Europe,Other countries, NorthAmerica,total, United States, Canada, Central America, total, ElSalvador, Guatemala, Honduras, Dominican Republic, Mexico, Panama, Costa Rica, Centra lAmerica,Othercoun, South America,total, Uruguay, Ecuador, Argentina, Bolivia, Brazil, Paraguay, Peru, Chile, Colombia, South America,Other countr, Oceania, total, Australia, NewZealand, Oceania,Other countries, Unclas sified countries</t>
   </si>
   <si>
     <t>Data Type: Original Data</t>
@@ -46,7 +46,7 @@
     <t>To year: 2025</t>
   </si>
   <si>
-    <t>To month: 11</t>
+    <t>To month: 12</t>
   </si>
   <si>
     <t>Period</t>
@@ -735,6 +735,9 @@
   <si>
     <t>2025-11</t>
   </si>
+  <si>
+    <t>2025-12</t>
+  </si>
 </sst>
 </file>
 
@@ -949,7 +952,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Picture 691d9f99-70b9-4a41-9ac2-321645e038aa"/>
+        <xdr:cNvPr id="1" name="Picture c7b46d57-52d3-4f5f-a544-9c6d35f454c4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -17253,115 +17256,444 @@
       </c>
     </row>
     <row r="69" s="1">
-      <c r="A69" s="6"/>
-      <c r="B69" s="6"/>
-      <c r="C69" s="6"/>
-      <c r="D69" s="6"/>
-      <c r="E69" s="6"/>
-      <c r="F69" s="6"/>
-      <c r="G69" s="6"/>
-      <c r="H69" s="6"/>
-      <c r="I69" s="6"/>
-      <c r="J69" s="6"/>
-      <c r="K69" s="6"/>
-      <c r="L69" s="6"/>
-      <c r="M69" s="6"/>
-      <c r="N69" s="6"/>
-      <c r="O69" s="6"/>
-      <c r="P69" s="6"/>
-      <c r="Q69" s="6"/>
-      <c r="R69" s="6"/>
-      <c r="S69" s="6"/>
-      <c r="T69" s="6"/>
-      <c r="U69" s="6"/>
-      <c r="V69" s="6"/>
-      <c r="W69" s="6"/>
-      <c r="X69" s="6"/>
-      <c r="Y69" s="6"/>
-      <c r="Z69" s="6"/>
-      <c r="AA69" s="6"/>
-      <c r="AB69" s="6"/>
-      <c r="AC69" s="6"/>
-      <c r="AD69" s="6"/>
-      <c r="AE69" s="6"/>
-      <c r="AF69" s="6"/>
-      <c r="AG69" s="6"/>
-      <c r="AH69" s="6"/>
-      <c r="AI69" s="6"/>
-      <c r="AJ69" s="6"/>
-      <c r="AK69" s="6"/>
-      <c r="AL69" s="6"/>
-      <c r="AM69" s="6"/>
-      <c r="AN69" s="6"/>
-      <c r="AO69" s="6"/>
-      <c r="AP69" s="6"/>
-      <c r="AQ69" s="6"/>
-      <c r="AR69" s="6"/>
-      <c r="AS69" s="6"/>
-      <c r="AT69" s="6"/>
-      <c r="AU69" s="6"/>
-      <c r="AV69" s="6"/>
-      <c r="AW69" s="6"/>
-      <c r="AX69" s="6"/>
-      <c r="AY69" s="6"/>
-      <c r="AZ69" s="6"/>
-      <c r="BA69" s="6"/>
-      <c r="BB69" s="6"/>
-      <c r="BC69" s="6"/>
-      <c r="BD69" s="6"/>
-      <c r="BE69" s="6"/>
-      <c r="BF69" s="6"/>
-      <c r="BG69" s="6"/>
-      <c r="BH69" s="6"/>
-      <c r="BI69" s="6"/>
-      <c r="BJ69" s="6"/>
-      <c r="BK69" s="6"/>
-      <c r="BL69" s="6"/>
-      <c r="BM69" s="6"/>
-      <c r="BN69" s="6"/>
-      <c r="BO69" s="6"/>
-      <c r="BP69" s="6"/>
-      <c r="BQ69" s="6"/>
-      <c r="BR69" s="6"/>
-      <c r="BS69" s="6"/>
-      <c r="BT69" s="6"/>
-      <c r="BU69" s="6"/>
-      <c r="BV69" s="6"/>
-      <c r="BW69" s="6"/>
-      <c r="BX69" s="6"/>
-      <c r="BY69" s="6"/>
-      <c r="BZ69" s="6"/>
-      <c r="CA69" s="6"/>
-      <c r="CB69" s="6"/>
-      <c r="CC69" s="6"/>
-      <c r="CD69" s="6"/>
-      <c r="CE69" s="6"/>
-      <c r="CF69" s="6"/>
-      <c r="CG69" s="6"/>
-      <c r="CH69" s="6"/>
-      <c r="CI69" s="6"/>
-      <c r="CJ69" s="6"/>
-      <c r="CK69" s="6"/>
-      <c r="CL69" s="6"/>
-      <c r="CM69" s="6"/>
-      <c r="CN69" s="6"/>
-      <c r="CO69" s="6"/>
-      <c r="CP69" s="6"/>
-      <c r="CQ69" s="6"/>
-      <c r="CR69" s="6"/>
-      <c r="CS69" s="6"/>
-      <c r="CT69" s="6"/>
-      <c r="CU69" s="6"/>
-      <c r="CV69" s="6"/>
-      <c r="CW69" s="6"/>
-      <c r="CX69" s="6"/>
-      <c r="CY69" s="6"/>
-      <c r="CZ69" s="6"/>
-      <c r="DA69" s="6"/>
-      <c r="DB69" s="6"/>
-      <c r="DC69" s="6"/>
-      <c r="DD69" s="6"/>
-      <c r="DE69" s="6"/>
+      <c r="A69" t="s" s="6">
+        <v>167</v>
+      </c>
+      <c r="B69" s="7">
+        <v>9.6</v>
+      </c>
+      <c r="C69" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="D69" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E69" s="7">
+        <v>0</v>
+      </c>
+      <c r="F69" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="G69" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="H69" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="I69" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="J69" s="7">
+        <v>0</v>
+      </c>
+      <c r="K69" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="L69" s="7">
+        <v>0</v>
+      </c>
+      <c r="M69" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="N69" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="O69" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="P69" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="Q69" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="R69" s="7">
+        <v>0</v>
+      </c>
+      <c r="S69" s="7">
+        <v>1</v>
+      </c>
+      <c r="T69" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="U69" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="V69" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="W69" s="7">
+        <v>0</v>
+      </c>
+      <c r="X69" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="Y69" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="Z69" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA69" s="7">
+        <v>3.4</v>
+      </c>
+      <c r="AB69" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC69" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="AD69" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE69" s="7">
+        <v>2.1</v>
+      </c>
+      <c r="AF69" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG69" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH69" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="AI69" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ69" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="AK69" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="AL69" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AM69" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="AN69" s="7">
+        <v>0</v>
+      </c>
+      <c r="AO69" s="7">
+        <v>0</v>
+      </c>
+      <c r="AP69" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="AQ69" s="7">
+        <v>63.4</v>
+      </c>
+      <c r="AR69" s="7">
+        <v>1.1</v>
+      </c>
+      <c r="AS69" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="AT69" s="7">
+        <v>3.7</v>
+      </c>
+      <c r="AU69" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="AV69" s="7">
+        <v>0</v>
+      </c>
+      <c r="AW69" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="AX69" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AY69" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="AZ69" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="BA69" s="7">
+        <v>5.1</v>
+      </c>
+      <c r="BB69" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="BC69" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="BD69" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="BE69" s="7">
+        <v>10</v>
+      </c>
+      <c r="BF69" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="BG69" s="7">
+        <v>0</v>
+      </c>
+      <c r="BH69" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="BI69" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="BJ69" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="BK69" s="7">
+        <v>0</v>
+      </c>
+      <c r="BL69" s="7">
+        <v>0</v>
+      </c>
+      <c r="BM69" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="BN69" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="BO69" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="BP69" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="BQ69" s="7">
+        <v>2.1</v>
+      </c>
+      <c r="BR69" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="BS69" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="BT69" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="BU69" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="BV69" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="BW69" s="7">
+        <v>17.9</v>
+      </c>
+      <c r="BX69" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="BY69" s="7">
+        <v>2.4</v>
+      </c>
+      <c r="BZ69" s="7">
+        <v>6.2</v>
+      </c>
+      <c r="CA69" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="CB69" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="CC69" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="CD69" s="7">
+        <v>52.1</v>
+      </c>
+      <c r="CE69" s="7">
+        <v>48.3</v>
+      </c>
+      <c r="CF69" s="7">
+        <v>3.7</v>
+      </c>
+      <c r="CG69" s="7">
+        <v>2.6</v>
+      </c>
+      <c r="CH69" s="7">
+        <v>0</v>
+      </c>
+      <c r="CI69" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="CJ69" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="CK69" s="7">
+        <v>0</v>
+      </c>
+      <c r="CL69" s="7">
+        <v>1.9</v>
+      </c>
+      <c r="CM69" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="CN69" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="CO69" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="CP69" s="7">
+        <v>5.2</v>
+      </c>
+      <c r="CQ69" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="CR69" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="CS69" s="7">
+        <v>1.7</v>
+      </c>
+      <c r="CT69" s="7">
+        <v>0</v>
+      </c>
+      <c r="CU69" s="7">
+        <v>2.4</v>
+      </c>
+      <c r="CV69" s="7">
+        <v>0</v>
+      </c>
+      <c r="CW69" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="CX69" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="CY69" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="CZ69" s="7">
+        <v>0</v>
+      </c>
+      <c r="DA69" s="7">
+        <v>2.3</v>
+      </c>
+      <c r="DB69" s="7">
+        <v>2.1</v>
+      </c>
+      <c r="DC69" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="DD69" s="7">
+        <v>0</v>
+      </c>
+      <c r="DE69" s="7">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="70" s="1">
+      <c r="A70" s="6"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="6"/>
+      <c r="J70" s="6"/>
+      <c r="K70" s="6"/>
+      <c r="L70" s="6"/>
+      <c r="M70" s="6"/>
+      <c r="N70" s="6"/>
+      <c r="O70" s="6"/>
+      <c r="P70" s="6"/>
+      <c r="Q70" s="6"/>
+      <c r="R70" s="6"/>
+      <c r="S70" s="6"/>
+      <c r="T70" s="6"/>
+      <c r="U70" s="6"/>
+      <c r="V70" s="6"/>
+      <c r="W70" s="6"/>
+      <c r="X70" s="6"/>
+      <c r="Y70" s="6"/>
+      <c r="Z70" s="6"/>
+      <c r="AA70" s="6"/>
+      <c r="AB70" s="6"/>
+      <c r="AC70" s="6"/>
+      <c r="AD70" s="6"/>
+      <c r="AE70" s="6"/>
+      <c r="AF70" s="6"/>
+      <c r="AG70" s="6"/>
+      <c r="AH70" s="6"/>
+      <c r="AI70" s="6"/>
+      <c r="AJ70" s="6"/>
+      <c r="AK70" s="6"/>
+      <c r="AL70" s="6"/>
+      <c r="AM70" s="6"/>
+      <c r="AN70" s="6"/>
+      <c r="AO70" s="6"/>
+      <c r="AP70" s="6"/>
+      <c r="AQ70" s="6"/>
+      <c r="AR70" s="6"/>
+      <c r="AS70" s="6"/>
+      <c r="AT70" s="6"/>
+      <c r="AU70" s="6"/>
+      <c r="AV70" s="6"/>
+      <c r="AW70" s="6"/>
+      <c r="AX70" s="6"/>
+      <c r="AY70" s="6"/>
+      <c r="AZ70" s="6"/>
+      <c r="BA70" s="6"/>
+      <c r="BB70" s="6"/>
+      <c r="BC70" s="6"/>
+      <c r="BD70" s="6"/>
+      <c r="BE70" s="6"/>
+      <c r="BF70" s="6"/>
+      <c r="BG70" s="6"/>
+      <c r="BH70" s="6"/>
+      <c r="BI70" s="6"/>
+      <c r="BJ70" s="6"/>
+      <c r="BK70" s="6"/>
+      <c r="BL70" s="6"/>
+      <c r="BM70" s="6"/>
+      <c r="BN70" s="6"/>
+      <c r="BO70" s="6"/>
+      <c r="BP70" s="6"/>
+      <c r="BQ70" s="6"/>
+      <c r="BR70" s="6"/>
+      <c r="BS70" s="6"/>
+      <c r="BT70" s="6"/>
+      <c r="BU70" s="6"/>
+      <c r="BV70" s="6"/>
+      <c r="BW70" s="6"/>
+      <c r="BX70" s="6"/>
+      <c r="BY70" s="6"/>
+      <c r="BZ70" s="6"/>
+      <c r="CA70" s="6"/>
+      <c r="CB70" s="6"/>
+      <c r="CC70" s="6"/>
+      <c r="CD70" s="6"/>
+      <c r="CE70" s="6"/>
+      <c r="CF70" s="6"/>
+      <c r="CG70" s="6"/>
+      <c r="CH70" s="6"/>
+      <c r="CI70" s="6"/>
+      <c r="CJ70" s="6"/>
+      <c r="CK70" s="6"/>
+      <c r="CL70" s="6"/>
+      <c r="CM70" s="6"/>
+      <c r="CN70" s="6"/>
+      <c r="CO70" s="6"/>
+      <c r="CP70" s="6"/>
+      <c r="CQ70" s="6"/>
+      <c r="CR70" s="6"/>
+      <c r="CS70" s="6"/>
+      <c r="CT70" s="6"/>
+      <c r="CU70" s="6"/>
+      <c r="CV70" s="6"/>
+      <c r="CW70" s="6"/>
+      <c r="CX70" s="6"/>
+      <c r="CY70" s="6"/>
+      <c r="CZ70" s="6"/>
+      <c r="DA70" s="6"/>
+      <c r="DB70" s="6"/>
+      <c r="DC70" s="6"/>
+      <c r="DD70" s="6"/>
+      <c r="DE70" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>